<commit_message>
Atualização planilhamento de Conferência
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_PEV.xlsx
+++ b/Documentação/Planilhas/Conferencia_PEV.xlsx
@@ -2662,8 +2662,19 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2692,6 +2703,18 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2704,37 +2727,36 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2771,28 +2793,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3226,10 +3226,10 @@
       <c r="BC1" s="1"/>
     </row>
     <row r="2" spans="1:58" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
@@ -3238,10 +3238,10 @@
       <c r="BC2" s="1"/>
     </row>
     <row r="3" spans="1:58" ht="21">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="5" t="s">
         <v>155</v>
       </c>
@@ -5180,66 +5180,66 @@
       <c r="BF17" s="3"/>
     </row>
     <row r="18" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="29" t="s">
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="30"/>
-      <c r="AC18" s="30"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="30"/>
-      <c r="AF18" s="30"/>
-      <c r="AG18" s="30"/>
-      <c r="AH18" s="30"/>
-      <c r="AI18" s="30"/>
-      <c r="AJ18" s="30"/>
-      <c r="AK18" s="30"/>
-      <c r="AL18" s="30"/>
-      <c r="AM18" s="30"/>
-      <c r="AN18" s="30"/>
-      <c r="AO18" s="30"/>
-      <c r="AP18" s="30"/>
-      <c r="AQ18" s="30"/>
-      <c r="AR18" s="30"/>
-      <c r="AS18" s="30"/>
-      <c r="AT18" s="30"/>
-      <c r="AU18" s="30"/>
-      <c r="AV18" s="30"/>
-      <c r="AW18" s="30"/>
-      <c r="AX18" s="30"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="41" t="s">
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="35"/>
+      <c r="AC18" s="35"/>
+      <c r="AD18" s="35"/>
+      <c r="AE18" s="35"/>
+      <c r="AF18" s="35"/>
+      <c r="AG18" s="35"/>
+      <c r="AH18" s="35"/>
+      <c r="AI18" s="35"/>
+      <c r="AJ18" s="35"/>
+      <c r="AK18" s="35"/>
+      <c r="AL18" s="35"/>
+      <c r="AM18" s="35"/>
+      <c r="AN18" s="35"/>
+      <c r="AO18" s="35"/>
+      <c r="AP18" s="35"/>
+      <c r="AQ18" s="35"/>
+      <c r="AR18" s="35"/>
+      <c r="AS18" s="35"/>
+      <c r="AT18" s="35"/>
+      <c r="AU18" s="35"/>
+      <c r="AV18" s="35"/>
+      <c r="AW18" s="35"/>
+      <c r="AX18" s="35"/>
+      <c r="AY18" s="36"/>
+      <c r="AZ18" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="BA18" s="41"/>
-      <c r="BB18" s="40" t="s">
+      <c r="BA18" s="50"/>
+      <c r="BB18" s="49" t="s">
         <v>104</v>
       </c>
       <c r="BC18" s="1"/>
@@ -5247,640 +5247,640 @@
       <c r="BF18" s="3"/>
     </row>
     <row r="19" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
-      <c r="S19" s="33"/>
-      <c r="T19" s="33"/>
-      <c r="U19" s="33"/>
-      <c r="V19" s="33"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="32"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="33"/>
-      <c r="AA19" s="33"/>
-      <c r="AB19" s="33"/>
-      <c r="AC19" s="33"/>
-      <c r="AD19" s="33"/>
-      <c r="AE19" s="33"/>
-      <c r="AF19" s="33"/>
-      <c r="AG19" s="33"/>
-      <c r="AH19" s="33"/>
-      <c r="AI19" s="33"/>
-      <c r="AJ19" s="33"/>
-      <c r="AK19" s="33"/>
-      <c r="AL19" s="33"/>
-      <c r="AM19" s="33"/>
-      <c r="AN19" s="33"/>
-      <c r="AO19" s="33"/>
-      <c r="AP19" s="33"/>
-      <c r="AQ19" s="33"/>
-      <c r="AR19" s="33"/>
-      <c r="AS19" s="33"/>
-      <c r="AT19" s="33"/>
-      <c r="AU19" s="33"/>
-      <c r="AV19" s="33"/>
-      <c r="AW19" s="33"/>
-      <c r="AX19" s="33"/>
-      <c r="AY19" s="34"/>
-      <c r="AZ19" s="41"/>
-      <c r="BA19" s="41"/>
-      <c r="BB19" s="40"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="39"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38"/>
+      <c r="AJ19" s="38"/>
+      <c r="AK19" s="38"/>
+      <c r="AL19" s="38"/>
+      <c r="AM19" s="38"/>
+      <c r="AN19" s="38"/>
+      <c r="AO19" s="38"/>
+      <c r="AP19" s="38"/>
+      <c r="AQ19" s="38"/>
+      <c r="AR19" s="38"/>
+      <c r="AS19" s="38"/>
+      <c r="AT19" s="38"/>
+      <c r="AU19" s="38"/>
+      <c r="AV19" s="38"/>
+      <c r="AW19" s="38"/>
+      <c r="AX19" s="38"/>
+      <c r="AY19" s="39"/>
+      <c r="AZ19" s="50"/>
+      <c r="BA19" s="50"/>
+      <c r="BB19" s="49"/>
       <c r="BC19" s="1"/>
       <c r="BE19" s="3"/>
       <c r="BF19" s="3"/>
     </row>
     <row r="20" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
-      <c r="AA20" s="36"/>
-      <c r="AB20" s="36"/>
-      <c r="AC20" s="36"/>
-      <c r="AD20" s="36"/>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="36"/>
-      <c r="AG20" s="36"/>
-      <c r="AH20" s="36"/>
-      <c r="AI20" s="36"/>
-      <c r="AJ20" s="36"/>
-      <c r="AK20" s="36"/>
-      <c r="AL20" s="36"/>
-      <c r="AM20" s="36"/>
-      <c r="AN20" s="36"/>
-      <c r="AO20" s="36"/>
-      <c r="AP20" s="36"/>
-      <c r="AQ20" s="36"/>
-      <c r="AR20" s="36"/>
-      <c r="AS20" s="36"/>
-      <c r="AT20" s="36"/>
-      <c r="AU20" s="36"/>
-      <c r="AV20" s="36"/>
-      <c r="AW20" s="36"/>
-      <c r="AX20" s="36"/>
-      <c r="AY20" s="37"/>
-      <c r="AZ20" s="41"/>
-      <c r="BA20" s="41"/>
-      <c r="BB20" s="40"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="42"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="41"/>
+      <c r="AB20" s="41"/>
+      <c r="AC20" s="41"/>
+      <c r="AD20" s="41"/>
+      <c r="AE20" s="41"/>
+      <c r="AF20" s="41"/>
+      <c r="AG20" s="41"/>
+      <c r="AH20" s="41"/>
+      <c r="AI20" s="41"/>
+      <c r="AJ20" s="41"/>
+      <c r="AK20" s="41"/>
+      <c r="AL20" s="41"/>
+      <c r="AM20" s="41"/>
+      <c r="AN20" s="41"/>
+      <c r="AO20" s="41"/>
+      <c r="AP20" s="41"/>
+      <c r="AQ20" s="41"/>
+      <c r="AR20" s="41"/>
+      <c r="AS20" s="41"/>
+      <c r="AT20" s="41"/>
+      <c r="AU20" s="41"/>
+      <c r="AV20" s="41"/>
+      <c r="AW20" s="41"/>
+      <c r="AX20" s="41"/>
+      <c r="AY20" s="42"/>
+      <c r="AZ20" s="50"/>
+      <c r="BA20" s="50"/>
+      <c r="BB20" s="49"/>
       <c r="BC20" s="1"/>
       <c r="BE20" s="3"/>
       <c r="BF20" s="3"/>
     </row>
     <row r="21" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="H21" s="42" t="s">
+      <c r="H21" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="I21" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="K21" s="42" t="s">
+      <c r="K21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="L21" s="42" t="s">
+      <c r="L21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="M21" s="42" t="s">
+      <c r="M21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="N21" s="42" t="s">
+      <c r="N21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="O21" s="42" t="s">
+      <c r="O21" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="P21" s="45" t="s">
+      <c r="P21" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="Q21" s="45" t="s">
+      <c r="Q21" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="R21" s="42" t="s">
+      <c r="R21" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="S21" s="42" t="s">
+      <c r="S21" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="T21" s="42" t="s">
+      <c r="T21" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="U21" s="42" t="s">
+      <c r="U21" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="V21" s="45" t="s">
+      <c r="V21" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="W21" s="42" t="s">
+      <c r="W21" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="X21" s="28" t="s">
+      <c r="X21" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="Y21" s="28" t="s">
+      <c r="Y21" s="46" t="s">
         <v>246</v>
       </c>
-      <c r="Z21" s="28"/>
-      <c r="AA21" s="28" t="s">
+      <c r="Z21" s="46"/>
+      <c r="AA21" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="AB21" s="28" t="s">
+      <c r="AB21" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="AC21" s="28" t="s">
+      <c r="AC21" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="AD21" s="28" t="s">
+      <c r="AD21" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="AE21" s="28" t="s">
+      <c r="AE21" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="AF21" s="28" t="s">
+      <c r="AF21" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="AG21" s="28" t="s">
+      <c r="AG21" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="AH21" s="28" t="s">
+      <c r="AH21" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="AI21" s="28" t="s">
+      <c r="AI21" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="AJ21" s="28" t="s">
+      <c r="AJ21" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="AK21" s="28" t="s">
+      <c r="AK21" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="AL21" s="28" t="s">
+      <c r="AL21" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="AM21" s="28" t="s">
+      <c r="AM21" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="AN21" s="28" t="s">
+      <c r="AN21" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="AO21" s="28" t="s">
+      <c r="AO21" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="AP21" s="28" t="s">
+      <c r="AP21" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="AQ21" s="28" t="s">
+      <c r="AQ21" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="AR21" s="28" t="s">
+      <c r="AR21" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="AS21" s="28" t="s">
+      <c r="AS21" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="AT21" s="28" t="s">
+      <c r="AT21" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="AU21" s="28" t="s">
+      <c r="AU21" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="AV21" s="28" t="s">
+      <c r="AV21" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="AW21" s="28" t="s">
+      <c r="AW21" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="AX21" s="28" t="s">
+      <c r="AX21" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="AY21" s="28" t="s">
+      <c r="AY21" s="46" t="s">
         <v>148</v>
       </c>
-      <c r="AZ21" s="39" t="s">
+      <c r="AZ21" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="BA21" s="39" t="s">
+      <c r="BA21" s="48" t="s">
         <v>249</v>
       </c>
-      <c r="BB21" s="28" t="s">
+      <c r="BB21" s="46" t="s">
         <v>105</v>
       </c>
       <c r="BC21" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="BD21" s="38" t="s">
+      <c r="BD21" s="47" t="s">
         <v>145</v>
       </c>
       <c r="BE21" s="3"/>
       <c r="BF21" s="3"/>
     </row>
     <row r="22" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="43"/>
-      <c r="Q22" s="43"/>
-      <c r="R22" s="43"/>
-      <c r="S22" s="43"/>
-      <c r="T22" s="43"/>
-      <c r="U22" s="43"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="46"/>
-      <c r="X22" s="28"/>
-      <c r="Y22" s="28"/>
-      <c r="Z22" s="28"/>
-      <c r="AA22" s="28"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="28"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
-      <c r="AM22" s="28"/>
-      <c r="AN22" s="28"/>
-      <c r="AO22" s="28"/>
-      <c r="AP22" s="28"/>
-      <c r="AQ22" s="28"/>
-      <c r="AR22" s="28"/>
-      <c r="AS22" s="28"/>
-      <c r="AT22" s="28"/>
-      <c r="AU22" s="28"/>
-      <c r="AV22" s="28"/>
-      <c r="AW22" s="28"/>
-      <c r="AX22" s="28"/>
-      <c r="AY22" s="28"/>
-      <c r="AZ22" s="39"/>
-      <c r="BA22" s="39"/>
-      <c r="BB22" s="28"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="46"/>
+      <c r="Z22" s="46"/>
+      <c r="AA22" s="46"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="46"/>
+      <c r="AD22" s="46"/>
+      <c r="AE22" s="46"/>
+      <c r="AF22" s="46"/>
+      <c r="AG22" s="46"/>
+      <c r="AH22" s="46"/>
+      <c r="AI22" s="46"/>
+      <c r="AJ22" s="46"/>
+      <c r="AK22" s="46"/>
+      <c r="AL22" s="46"/>
+      <c r="AM22" s="46"/>
+      <c r="AN22" s="46"/>
+      <c r="AO22" s="46"/>
+      <c r="AP22" s="46"/>
+      <c r="AQ22" s="46"/>
+      <c r="AR22" s="46"/>
+      <c r="AS22" s="46"/>
+      <c r="AT22" s="46"/>
+      <c r="AU22" s="46"/>
+      <c r="AV22" s="46"/>
+      <c r="AW22" s="46"/>
+      <c r="AX22" s="46"/>
+      <c r="AY22" s="46"/>
+      <c r="AZ22" s="48"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="46"/>
       <c r="BC22" s="27"/>
-      <c r="BD22" s="38"/>
+      <c r="BD22" s="47"/>
     </row>
     <row r="23" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A23" s="43"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-      <c r="AG23" s="28"/>
-      <c r="AH23" s="28"/>
-      <c r="AI23" s="28"/>
-      <c r="AJ23" s="28"/>
-      <c r="AK23" s="28"/>
-      <c r="AL23" s="28"/>
-      <c r="AM23" s="28"/>
-      <c r="AN23" s="28"/>
-      <c r="AO23" s="28"/>
-      <c r="AP23" s="28"/>
-      <c r="AQ23" s="28"/>
-      <c r="AR23" s="28"/>
-      <c r="AS23" s="28"/>
-      <c r="AT23" s="28"/>
-      <c r="AU23" s="28"/>
-      <c r="AV23" s="28"/>
-      <c r="AW23" s="28"/>
-      <c r="AX23" s="28"/>
-      <c r="AY23" s="28"/>
-      <c r="AZ23" s="39"/>
-      <c r="BA23" s="39"/>
-      <c r="BB23" s="28"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="46"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="46"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="46"/>
+      <c r="AE23" s="46"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="46"/>
+      <c r="AH23" s="46"/>
+      <c r="AI23" s="46"/>
+      <c r="AJ23" s="46"/>
+      <c r="AK23" s="46"/>
+      <c r="AL23" s="46"/>
+      <c r="AM23" s="46"/>
+      <c r="AN23" s="46"/>
+      <c r="AO23" s="46"/>
+      <c r="AP23" s="46"/>
+      <c r="AQ23" s="46"/>
+      <c r="AR23" s="46"/>
+      <c r="AS23" s="46"/>
+      <c r="AT23" s="46"/>
+      <c r="AU23" s="46"/>
+      <c r="AV23" s="46"/>
+      <c r="AW23" s="46"/>
+      <c r="AX23" s="46"/>
+      <c r="AY23" s="46"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="46"/>
       <c r="BC23" s="27"/>
-      <c r="BD23" s="38"/>
+      <c r="BD23" s="47"/>
     </row>
     <row r="24" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A24" s="43"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="46"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
-      <c r="AG24" s="28"/>
-      <c r="AH24" s="28"/>
-      <c r="AI24" s="28"/>
-      <c r="AJ24" s="28"/>
-      <c r="AK24" s="28"/>
-      <c r="AL24" s="28"/>
-      <c r="AM24" s="28"/>
-      <c r="AN24" s="28"/>
-      <c r="AO24" s="28"/>
-      <c r="AP24" s="28"/>
-      <c r="AQ24" s="28"/>
-      <c r="AR24" s="28"/>
-      <c r="AS24" s="28"/>
-      <c r="AT24" s="28"/>
-      <c r="AU24" s="28"/>
-      <c r="AV24" s="28"/>
-      <c r="AW24" s="28"/>
-      <c r="AX24" s="28"/>
-      <c r="AY24" s="28"/>
-      <c r="AZ24" s="39"/>
-      <c r="BA24" s="39"/>
-      <c r="BB24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="46"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="46"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
+      <c r="AD24" s="46"/>
+      <c r="AE24" s="46"/>
+      <c r="AF24" s="46"/>
+      <c r="AG24" s="46"/>
+      <c r="AH24" s="46"/>
+      <c r="AI24" s="46"/>
+      <c r="AJ24" s="46"/>
+      <c r="AK24" s="46"/>
+      <c r="AL24" s="46"/>
+      <c r="AM24" s="46"/>
+      <c r="AN24" s="46"/>
+      <c r="AO24" s="46"/>
+      <c r="AP24" s="46"/>
+      <c r="AQ24" s="46"/>
+      <c r="AR24" s="46"/>
+      <c r="AS24" s="46"/>
+      <c r="AT24" s="46"/>
+      <c r="AU24" s="46"/>
+      <c r="AV24" s="46"/>
+      <c r="AW24" s="46"/>
+      <c r="AX24" s="46"/>
+      <c r="AY24" s="46"/>
+      <c r="AZ24" s="48"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="46"/>
       <c r="BC24" s="27"/>
-      <c r="BD24" s="38"/>
+      <c r="BD24" s="47"/>
     </row>
     <row r="25" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A25" s="43"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
-      <c r="T25" s="43"/>
-      <c r="U25" s="43"/>
-      <c r="V25" s="43"/>
-      <c r="W25" s="46"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="28"/>
-      <c r="AI25" s="28"/>
-      <c r="AJ25" s="28"/>
-      <c r="AK25" s="28"/>
-      <c r="AL25" s="28"/>
-      <c r="AM25" s="28"/>
-      <c r="AN25" s="28"/>
-      <c r="AO25" s="28"/>
-      <c r="AP25" s="28"/>
-      <c r="AQ25" s="28"/>
-      <c r="AR25" s="28"/>
-      <c r="AS25" s="28"/>
-      <c r="AT25" s="28"/>
-      <c r="AU25" s="28"/>
-      <c r="AV25" s="28"/>
-      <c r="AW25" s="28"/>
-      <c r="AX25" s="28"/>
-      <c r="AY25" s="28"/>
-      <c r="AZ25" s="39"/>
-      <c r="BA25" s="39"/>
-      <c r="BB25" s="28"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="46"/>
+      <c r="Z25" s="46"/>
+      <c r="AA25" s="46"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46"/>
+      <c r="AD25" s="46"/>
+      <c r="AE25" s="46"/>
+      <c r="AF25" s="46"/>
+      <c r="AG25" s="46"/>
+      <c r="AH25" s="46"/>
+      <c r="AI25" s="46"/>
+      <c r="AJ25" s="46"/>
+      <c r="AK25" s="46"/>
+      <c r="AL25" s="46"/>
+      <c r="AM25" s="46"/>
+      <c r="AN25" s="46"/>
+      <c r="AO25" s="46"/>
+      <c r="AP25" s="46"/>
+      <c r="AQ25" s="46"/>
+      <c r="AR25" s="46"/>
+      <c r="AS25" s="46"/>
+      <c r="AT25" s="46"/>
+      <c r="AU25" s="46"/>
+      <c r="AV25" s="46"/>
+      <c r="AW25" s="46"/>
+      <c r="AX25" s="46"/>
+      <c r="AY25" s="46"/>
+      <c r="AZ25" s="48"/>
+      <c r="BA25" s="48"/>
+      <c r="BB25" s="46"/>
       <c r="BC25" s="27"/>
-      <c r="BD25" s="38"/>
+      <c r="BD25" s="47"/>
     </row>
     <row r="26" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A26" s="43"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
-      <c r="T26" s="43"/>
-      <c r="U26" s="43"/>
-      <c r="V26" s="43"/>
-      <c r="W26" s="46"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="28"/>
-      <c r="AH26" s="28"/>
-      <c r="AI26" s="28"/>
-      <c r="AJ26" s="28"/>
-      <c r="AK26" s="28"/>
-      <c r="AL26" s="28"/>
-      <c r="AM26" s="28"/>
-      <c r="AN26" s="28"/>
-      <c r="AO26" s="28"/>
-      <c r="AP26" s="28"/>
-      <c r="AQ26" s="28"/>
-      <c r="AR26" s="28"/>
-      <c r="AS26" s="28"/>
-      <c r="AT26" s="28"/>
-      <c r="AU26" s="28"/>
-      <c r="AV26" s="28"/>
-      <c r="AW26" s="28"/>
-      <c r="AX26" s="28"/>
-      <c r="AY26" s="28"/>
-      <c r="AZ26" s="39"/>
-      <c r="BA26" s="39"/>
-      <c r="BB26" s="28"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="46"/>
+      <c r="Z26" s="46"/>
+      <c r="AA26" s="46"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="46"/>
+      <c r="AD26" s="46"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="46"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
+      <c r="AK26" s="46"/>
+      <c r="AL26" s="46"/>
+      <c r="AM26" s="46"/>
+      <c r="AN26" s="46"/>
+      <c r="AO26" s="46"/>
+      <c r="AP26" s="46"/>
+      <c r="AQ26" s="46"/>
+      <c r="AR26" s="46"/>
+      <c r="AS26" s="46"/>
+      <c r="AT26" s="46"/>
+      <c r="AU26" s="46"/>
+      <c r="AV26" s="46"/>
+      <c r="AW26" s="46"/>
+      <c r="AX26" s="46"/>
+      <c r="AY26" s="46"/>
+      <c r="AZ26" s="48"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="46"/>
       <c r="BC26" s="27"/>
-      <c r="BD26" s="38"/>
+      <c r="BD26" s="47"/>
     </row>
     <row r="27" spans="1:58" ht="11.25" customHeight="1">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="44"/>
-      <c r="T27" s="44"/>
-      <c r="U27" s="44"/>
-      <c r="V27" s="44"/>
-      <c r="W27" s="47"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
-      <c r="AA27" s="28"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="28"/>
-      <c r="AD27" s="28"/>
-      <c r="AE27" s="28"/>
-      <c r="AF27" s="28"/>
-      <c r="AG27" s="28"/>
-      <c r="AH27" s="28"/>
-      <c r="AI27" s="28"/>
-      <c r="AJ27" s="28"/>
-      <c r="AK27" s="28"/>
-      <c r="AL27" s="28"/>
-      <c r="AM27" s="28"/>
-      <c r="AN27" s="28"/>
-      <c r="AO27" s="28"/>
-      <c r="AP27" s="28"/>
-      <c r="AQ27" s="28"/>
-      <c r="AR27" s="28"/>
-      <c r="AS27" s="28"/>
-      <c r="AT27" s="28"/>
-      <c r="AU27" s="28"/>
-      <c r="AV27" s="28"/>
-      <c r="AW27" s="28"/>
-      <c r="AX27" s="28"/>
-      <c r="AY27" s="28"/>
-      <c r="AZ27" s="39"/>
-      <c r="BA27" s="39"/>
-      <c r="BB27" s="28"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="30"/>
+      <c r="W27" s="45"/>
+      <c r="X27" s="46"/>
+      <c r="Y27" s="46"/>
+      <c r="Z27" s="46"/>
+      <c r="AA27" s="46"/>
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="46"/>
+      <c r="AD27" s="46"/>
+      <c r="AE27" s="46"/>
+      <c r="AF27" s="46"/>
+      <c r="AG27" s="46"/>
+      <c r="AH27" s="46"/>
+      <c r="AI27" s="46"/>
+      <c r="AJ27" s="46"/>
+      <c r="AK27" s="46"/>
+      <c r="AL27" s="46"/>
+      <c r="AM27" s="46"/>
+      <c r="AN27" s="46"/>
+      <c r="AO27" s="46"/>
+      <c r="AP27" s="46"/>
+      <c r="AQ27" s="46"/>
+      <c r="AR27" s="46"/>
+      <c r="AS27" s="46"/>
+      <c r="AT27" s="46"/>
+      <c r="AU27" s="46"/>
+      <c r="AV27" s="46"/>
+      <c r="AW27" s="46"/>
+      <c r="AX27" s="46"/>
+      <c r="AY27" s="46"/>
+      <c r="AZ27" s="48"/>
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="46"/>
       <c r="BC27" s="27"/>
-      <c r="BD27" s="38"/>
+      <c r="BD27" s="47"/>
     </row>
     <row r="28" spans="1:58">
       <c r="L28" s="1"/>
@@ -6089,10 +6089,10 @@
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
       <c r="P36" s="27"/>
-      <c r="R36" s="50" t="s">
+      <c r="R36" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="S36" s="50" t="s">
+      <c r="S36" s="31" t="s">
         <v>253</v>
       </c>
       <c r="U36" s="27"/>
@@ -6105,8 +6105,8 @@
       <c r="E37" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="R37" s="50"/>
-      <c r="S37" s="50"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
       <c r="AW37" s="11" t="s">
         <v>139</v>
       </c>
@@ -6115,8 +6115,8 @@
       <c r="E38" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="R38" s="50"/>
-      <c r="S38" s="50"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="31"/>
       <c r="AQ38" s="11" t="s">
         <v>78</v>
       </c>
@@ -6128,8 +6128,8 @@
       <c r="E39" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="R39" s="50"/>
-      <c r="S39" s="50"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
       <c r="AQ39" s="11" t="s">
         <v>126</v>
       </c>
@@ -6138,8 +6138,8 @@
       </c>
     </row>
     <row r="40" spans="5:54">
-      <c r="R40" s="50"/>
-      <c r="S40" s="50"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="31"/>
       <c r="AQ40" s="11" t="s">
         <v>127</v>
       </c>
@@ -6148,44 +6148,44 @@
       </c>
     </row>
     <row r="41" spans="5:54">
-      <c r="R41" s="50"/>
-      <c r="S41" s="50"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
       <c r="AW41" s="11" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="42" spans="5:54">
-      <c r="R42" s="50"/>
-      <c r="S42" s="50"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
       <c r="AQ42" s="27" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="43" spans="5:54">
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
+      <c r="R43" s="31"/>
+      <c r="S43" s="31"/>
       <c r="AQ43" s="27"/>
     </row>
     <row r="44" spans="5:54">
-      <c r="R44" s="50"/>
-      <c r="S44" s="50"/>
+      <c r="R44" s="31"/>
+      <c r="S44" s="31"/>
       <c r="AQ44" s="27"/>
     </row>
     <row r="45" spans="5:54">
-      <c r="R45" s="50"/>
-      <c r="S45" s="50"/>
+      <c r="R45" s="31"/>
+      <c r="S45" s="31"/>
     </row>
     <row r="46" spans="5:54">
-      <c r="R46" s="50"/>
-      <c r="S46" s="50"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
     </row>
     <row r="47" spans="5:54">
-      <c r="R47" s="50"/>
-      <c r="S47" s="50"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
     </row>
     <row r="48" spans="5:54">
-      <c r="R48" s="50"/>
-      <c r="S48" s="50"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="31"/>
     </row>
     <row r="50" spans="18:19">
       <c r="R50" s="27" t="s">
@@ -6209,14 +6209,63 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="P29:P36"/>
-    <mergeCell ref="R50:R53"/>
-    <mergeCell ref="S21:S27"/>
-    <mergeCell ref="S29:S34"/>
-    <mergeCell ref="S36:S48"/>
-    <mergeCell ref="S50:S53"/>
-    <mergeCell ref="R29:R34"/>
-    <mergeCell ref="R36:R48"/>
+    <mergeCell ref="AQ42:AQ44"/>
+    <mergeCell ref="BB21:BB27"/>
+    <mergeCell ref="X18:AY20"/>
+    <mergeCell ref="BC21:BC27"/>
+    <mergeCell ref="BD21:BD27"/>
+    <mergeCell ref="AN21:AN27"/>
+    <mergeCell ref="AO21:AO27"/>
+    <mergeCell ref="AP21:AP27"/>
+    <mergeCell ref="AY21:AY27"/>
+    <mergeCell ref="AZ21:AZ27"/>
+    <mergeCell ref="BB18:BB20"/>
+    <mergeCell ref="BA21:BA27"/>
+    <mergeCell ref="AZ18:BA20"/>
+    <mergeCell ref="AW21:AW27"/>
+    <mergeCell ref="AX21:AX27"/>
+    <mergeCell ref="AE21:AE27"/>
+    <mergeCell ref="AF21:AF27"/>
+    <mergeCell ref="AK21:AK27"/>
+    <mergeCell ref="AM21:AM27"/>
+    <mergeCell ref="AL21:AL27"/>
+    <mergeCell ref="AJ21:AJ27"/>
+    <mergeCell ref="AQ21:AQ27"/>
+    <mergeCell ref="AH21:AH27"/>
+    <mergeCell ref="AG21:AG27"/>
+    <mergeCell ref="AQ29:AQ36"/>
+    <mergeCell ref="R21:R27"/>
+    <mergeCell ref="AI21:AI27"/>
+    <mergeCell ref="AC21:AC27"/>
+    <mergeCell ref="AB21:AB27"/>
+    <mergeCell ref="AA21:AA27"/>
+    <mergeCell ref="AD21:AD27"/>
+    <mergeCell ref="U29:U36"/>
+    <mergeCell ref="AV21:AV27"/>
+    <mergeCell ref="AU21:AU27"/>
+    <mergeCell ref="AR21:AR27"/>
+    <mergeCell ref="AT21:AT27"/>
+    <mergeCell ref="AS21:AS27"/>
+    <mergeCell ref="I29:I36"/>
+    <mergeCell ref="F29:F36"/>
+    <mergeCell ref="G29:G36"/>
+    <mergeCell ref="H29:H36"/>
+    <mergeCell ref="J21:J27"/>
+    <mergeCell ref="F21:F27"/>
+    <mergeCell ref="I21:I27"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="H21:H27"/>
+    <mergeCell ref="X21:X27"/>
+    <mergeCell ref="Y21:Z27"/>
+    <mergeCell ref="U21:U27"/>
+    <mergeCell ref="K29:K36"/>
+    <mergeCell ref="L21:L27"/>
+    <mergeCell ref="L29:L36"/>
+    <mergeCell ref="K21:K27"/>
+    <mergeCell ref="M29:M36"/>
+    <mergeCell ref="N21:N27"/>
+    <mergeCell ref="N29:N36"/>
+    <mergeCell ref="P21:P27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A21:A27"/>
@@ -6230,64 +6279,15 @@
     <mergeCell ref="Q21:Q27"/>
     <mergeCell ref="V21:V27"/>
     <mergeCell ref="W21:W27"/>
-    <mergeCell ref="X21:X27"/>
-    <mergeCell ref="Y21:Z27"/>
-    <mergeCell ref="U21:U27"/>
-    <mergeCell ref="K29:K36"/>
-    <mergeCell ref="L21:L27"/>
-    <mergeCell ref="L29:L36"/>
     <mergeCell ref="E21:E27"/>
-    <mergeCell ref="I29:I36"/>
-    <mergeCell ref="F29:F36"/>
-    <mergeCell ref="G29:G36"/>
-    <mergeCell ref="H29:H36"/>
-    <mergeCell ref="J21:J27"/>
-    <mergeCell ref="K21:K27"/>
-    <mergeCell ref="F21:F27"/>
-    <mergeCell ref="I21:I27"/>
-    <mergeCell ref="G21:G27"/>
-    <mergeCell ref="H21:H27"/>
-    <mergeCell ref="M29:M36"/>
-    <mergeCell ref="N21:N27"/>
-    <mergeCell ref="N29:N36"/>
-    <mergeCell ref="AV21:AV27"/>
-    <mergeCell ref="AU21:AU27"/>
-    <mergeCell ref="AR21:AR27"/>
-    <mergeCell ref="AT21:AT27"/>
-    <mergeCell ref="AS21:AS27"/>
-    <mergeCell ref="AQ29:AQ36"/>
-    <mergeCell ref="R21:R27"/>
-    <mergeCell ref="AI21:AI27"/>
-    <mergeCell ref="AC21:AC27"/>
-    <mergeCell ref="AB21:AB27"/>
-    <mergeCell ref="AA21:AA27"/>
-    <mergeCell ref="AD21:AD27"/>
-    <mergeCell ref="P21:P27"/>
-    <mergeCell ref="U29:U36"/>
-    <mergeCell ref="AW21:AW27"/>
-    <mergeCell ref="AX21:AX27"/>
-    <mergeCell ref="AE21:AE27"/>
-    <mergeCell ref="AF21:AF27"/>
-    <mergeCell ref="AK21:AK27"/>
-    <mergeCell ref="AM21:AM27"/>
-    <mergeCell ref="AL21:AL27"/>
-    <mergeCell ref="AJ21:AJ27"/>
-    <mergeCell ref="AQ21:AQ27"/>
-    <mergeCell ref="AH21:AH27"/>
-    <mergeCell ref="AG21:AG27"/>
-    <mergeCell ref="AQ42:AQ44"/>
-    <mergeCell ref="BB21:BB27"/>
-    <mergeCell ref="X18:AY20"/>
-    <mergeCell ref="BC21:BC27"/>
-    <mergeCell ref="BD21:BD27"/>
-    <mergeCell ref="AN21:AN27"/>
-    <mergeCell ref="AO21:AO27"/>
-    <mergeCell ref="AP21:AP27"/>
-    <mergeCell ref="AY21:AY27"/>
-    <mergeCell ref="AZ21:AZ27"/>
-    <mergeCell ref="BB18:BB20"/>
-    <mergeCell ref="BA21:BA27"/>
-    <mergeCell ref="AZ18:BA20"/>
+    <mergeCell ref="P29:P36"/>
+    <mergeCell ref="R50:R53"/>
+    <mergeCell ref="S21:S27"/>
+    <mergeCell ref="S29:S34"/>
+    <mergeCell ref="S36:S48"/>
+    <mergeCell ref="S50:S53"/>
+    <mergeCell ref="R29:R34"/>
+    <mergeCell ref="R36:R48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6370,10 +6370,10 @@
       <c r="BC1" s="1"/>
     </row>
     <row r="2" spans="1:58" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="5" t="s">
         <v>156</v>
       </c>
@@ -6381,10 +6381,10 @@
       <c r="BC2" s="1"/>
     </row>
     <row r="3" spans="1:58" ht="21">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="5" t="s">
         <v>190</v>
       </c>
@@ -6394,10 +6394,10 @@
       <c r="BC3" s="1"/>
     </row>
     <row r="4" spans="1:58" ht="33" customHeight="1">
-      <c r="U4" s="51" t="s">
+      <c r="U4" s="53" t="s">
         <v>612</v>
       </c>
-      <c r="V4" s="51"/>
+      <c r="V4" s="53"/>
       <c r="AW4" s="4"/>
     </row>
     <row r="6" spans="1:58" s="8" customFormat="1" ht="19.5" customHeight="1">
@@ -7498,373 +7498,373 @@
       </c>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53" t="s">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="53"/>
-      <c r="X19" s="53"/>
-      <c r="Y19" s="53"/>
-      <c r="Z19" s="53"/>
-      <c r="AA19" s="53"/>
-      <c r="AB19" s="53"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="51"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="53"/>
-      <c r="W20" s="53"/>
-      <c r="X20" s="53"/>
-      <c r="Y20" s="53"/>
-      <c r="Z20" s="53"/>
-      <c r="AA20" s="53"/>
-      <c r="AB20" s="53"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="53"/>
-      <c r="V21" s="53"/>
-      <c r="W21" s="53"/>
-      <c r="X21" s="53"/>
-      <c r="Y21" s="53"/>
-      <c r="Z21" s="53"/>
-      <c r="AA21" s="53"/>
-      <c r="AB21" s="53"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="51"/>
     </row>
     <row r="22" spans="1:29" ht="11.25" customHeight="1">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="L22" s="28" t="s">
+      <c r="L22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="M22" s="28" t="s">
+      <c r="M22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="N22" s="28" t="s">
+      <c r="N22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="O22" s="28" t="s">
+      <c r="O22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="Q22" s="28" t="s">
+      <c r="Q22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="R22" s="28" t="s">
+      <c r="R22" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="S22" s="28" t="s">
+      <c r="S22" s="46" t="s">
         <v>611</v>
       </c>
-      <c r="T22" s="28" t="s">
+      <c r="T22" s="46" t="s">
         <v>177</v>
       </c>
-      <c r="U22" s="28" t="s">
+      <c r="U22" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="V22" s="28" t="s">
+      <c r="V22" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="W22" s="28" t="s">
+      <c r="W22" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="X22" s="28" t="s">
+      <c r="X22" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="Y22" s="28" t="s">
+      <c r="Y22" s="46" t="s">
         <v>183</v>
       </c>
-      <c r="Z22" s="28" t="s">
+      <c r="Z22" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="AA22" s="28" t="s">
+      <c r="AA22" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="AB22" s="28" t="s">
+      <c r="AB22" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="AC22" s="39" t="s">
+      <c r="AC22" s="48" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:29">
-      <c r="A23" s="46"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="39"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="46"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="46"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="48"/>
     </row>
     <row r="24" spans="1:29">
-      <c r="A24" s="46"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="39"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="46"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="46"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="48"/>
     </row>
     <row r="25" spans="1:29">
-      <c r="A25" s="46"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="39"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="46"/>
+      <c r="Z25" s="46"/>
+      <c r="AA25" s="46"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="48"/>
     </row>
     <row r="26" spans="1:29">
-      <c r="A26" s="46"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="28"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="39"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="46"/>
+      <c r="Z26" s="46"/>
+      <c r="AA26" s="46"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="48"/>
     </row>
     <row r="27" spans="1:29">
-      <c r="A27" s="46"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
-      <c r="AA27" s="28"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="39"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
+      <c r="Y27" s="46"/>
+      <c r="Z27" s="46"/>
+      <c r="AA27" s="46"/>
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="48"/>
     </row>
     <row r="28" spans="1:29">
-      <c r="A28" s="47"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="28"/>
-      <c r="V28" s="28"/>
-      <c r="W28" s="28"/>
-      <c r="X28" s="28"/>
-      <c r="Y28" s="28"/>
-      <c r="Z28" s="28"/>
-      <c r="AA28" s="28"/>
-      <c r="AB28" s="28"/>
-      <c r="AC28" s="39"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="46"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="46"/>
+      <c r="Z28" s="46"/>
+      <c r="AA28" s="46"/>
+      <c r="AB28" s="46"/>
+      <c r="AC28" s="48"/>
     </row>
     <row r="29" spans="1:29">
       <c r="J29" s="1"/>
@@ -8053,6 +8053,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="Q30:Q37"/>
+    <mergeCell ref="AA22:AA28"/>
+    <mergeCell ref="R30:R37"/>
+    <mergeCell ref="R22:R28"/>
+    <mergeCell ref="J30:J37"/>
+    <mergeCell ref="X22:X28"/>
+    <mergeCell ref="O30:O37"/>
+    <mergeCell ref="M30:M37"/>
+    <mergeCell ref="N30:N37"/>
+    <mergeCell ref="P30:P37"/>
+    <mergeCell ref="M22:M28"/>
+    <mergeCell ref="N22:N28"/>
+    <mergeCell ref="O22:O28"/>
+    <mergeCell ref="J22:J28"/>
+    <mergeCell ref="P22:P28"/>
+    <mergeCell ref="V22:V28"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="K22:K28"/>
+    <mergeCell ref="L22:L28"/>
+    <mergeCell ref="L30:L37"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="D30:D37"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="F22:F28"/>
+    <mergeCell ref="I30:I37"/>
+    <mergeCell ref="E30:E37"/>
+    <mergeCell ref="F30:F37"/>
+    <mergeCell ref="G30:G37"/>
+    <mergeCell ref="H30:H37"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="AC22:AC28"/>
@@ -8069,39 +8102,6 @@
     <mergeCell ref="I22:I28"/>
     <mergeCell ref="G22:G28"/>
     <mergeCell ref="H22:H28"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="K22:K28"/>
-    <mergeCell ref="L22:L28"/>
-    <mergeCell ref="L30:L37"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="D30:D37"/>
-    <mergeCell ref="E22:E28"/>
-    <mergeCell ref="F22:F28"/>
-    <mergeCell ref="I30:I37"/>
-    <mergeCell ref="E30:E37"/>
-    <mergeCell ref="F30:F37"/>
-    <mergeCell ref="G30:G37"/>
-    <mergeCell ref="H30:H37"/>
-    <mergeCell ref="J30:J37"/>
-    <mergeCell ref="X22:X28"/>
-    <mergeCell ref="O30:O37"/>
-    <mergeCell ref="M30:M37"/>
-    <mergeCell ref="N30:N37"/>
-    <mergeCell ref="P30:P37"/>
-    <mergeCell ref="M22:M28"/>
-    <mergeCell ref="N22:N28"/>
-    <mergeCell ref="O22:O28"/>
-    <mergeCell ref="J22:J28"/>
-    <mergeCell ref="P22:P28"/>
-    <mergeCell ref="V22:V28"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="Q30:Q37"/>
-    <mergeCell ref="AA22:AA28"/>
-    <mergeCell ref="R30:R37"/>
-    <mergeCell ref="R22:R28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8116,7 +8116,7 @@
   <dimension ref="A1:BF46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG45" sqref="AG45"/>
+      <selection activeCell="G18" sqref="G18:W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -8185,10 +8185,10 @@
       <c r="BC1" s="1"/>
     </row>
     <row r="2" spans="1:58" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="5" t="s">
         <v>191</v>
       </c>
@@ -8219,10 +8219,10 @@
       <c r="BF2" s="3"/>
     </row>
     <row r="3" spans="1:58" ht="21">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="5" t="s">
         <v>285</v>
       </c>
@@ -9663,482 +9663,482 @@
       <c r="AH17" s="1"/>
     </row>
     <row r="18" spans="1:38" ht="11.25" customHeight="1">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="61" t="s">
         <v>284</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="57" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="65" t="s">
         <v>261</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="56" t="s">
+      <c r="H18" s="66"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
+      <c r="S18" s="66"/>
+      <c r="T18" s="66"/>
+      <c r="U18" s="66"/>
+      <c r="V18" s="66"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="Y18" s="56"/>
-      <c r="Z18" s="56"/>
-      <c r="AA18" s="56"/>
-      <c r="AB18" s="56"/>
-      <c r="AC18" s="56"/>
-      <c r="AD18" s="56"/>
-      <c r="AE18" s="56"/>
-      <c r="AF18" s="56"/>
-      <c r="AG18" s="56"/>
-      <c r="AH18" s="54" t="s">
+      <c r="Y18" s="64"/>
+      <c r="Z18" s="64"/>
+      <c r="AA18" s="64"/>
+      <c r="AB18" s="64"/>
+      <c r="AC18" s="64"/>
+      <c r="AD18" s="64"/>
+      <c r="AE18" s="64"/>
+      <c r="AF18" s="64"/>
+      <c r="AG18" s="64"/>
+      <c r="AH18" s="62" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:38" ht="11.25" customHeight="1">
-      <c r="A19" s="71"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="R19" s="61"/>
-      <c r="S19" s="61"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="62"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="56"/>
-      <c r="AC19" s="56"/>
-      <c r="AD19" s="56"/>
-      <c r="AE19" s="56"/>
-      <c r="AF19" s="56"/>
-      <c r="AG19" s="56"/>
-      <c r="AH19" s="54"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="69"/>
+      <c r="W19" s="70"/>
+      <c r="X19" s="64"/>
+      <c r="Y19" s="64"/>
+      <c r="Z19" s="64"/>
+      <c r="AA19" s="64"/>
+      <c r="AB19" s="64"/>
+      <c r="AC19" s="64"/>
+      <c r="AD19" s="64"/>
+      <c r="AE19" s="64"/>
+      <c r="AF19" s="64"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="62"/>
       <c r="AI19" s="1"/>
     </row>
     <row r="20" spans="1:38" ht="11.25" customHeight="1">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="64"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="64"/>
-      <c r="S20" s="64"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
-      <c r="W20" s="65"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
-      <c r="AC20" s="56"/>
-      <c r="AD20" s="56"/>
-      <c r="AE20" s="56"/>
-      <c r="AF20" s="56"/>
-      <c r="AG20" s="56"/>
-      <c r="AH20" s="54"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="72"/>
+      <c r="Q20" s="72"/>
+      <c r="R20" s="72"/>
+      <c r="S20" s="72"/>
+      <c r="T20" s="72"/>
+      <c r="U20" s="72"/>
+      <c r="V20" s="72"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="64"/>
+      <c r="Y20" s="64"/>
+      <c r="Z20" s="64"/>
+      <c r="AA20" s="64"/>
+      <c r="AB20" s="64"/>
+      <c r="AC20" s="64"/>
+      <c r="AD20" s="64"/>
+      <c r="AE20" s="64"/>
+      <c r="AF20" s="64"/>
+      <c r="AG20" s="64"/>
+      <c r="AH20" s="62"/>
       <c r="AI20" s="1"/>
     </row>
     <row r="21" spans="1:38" ht="11.25" customHeight="1">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="44" t="s">
         <v>232</v>
       </c>
-      <c r="H21" s="46" t="s">
+      <c r="H21" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="J21" s="46" t="s">
+      <c r="J21" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="K21" s="46" t="s">
+      <c r="K21" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="M21" s="46" t="s">
+      <c r="M21" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="N21" s="46" t="s">
+      <c r="N21" s="44" t="s">
         <v>225</v>
       </c>
-      <c r="O21" s="47" t="s">
+      <c r="O21" s="45" t="s">
         <v>270</v>
       </c>
-      <c r="P21" s="47" t="s">
+      <c r="P21" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="Q21" s="47" t="s">
+      <c r="Q21" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="R21" s="47" t="s">
+      <c r="R21" s="45" t="s">
         <v>264</v>
       </c>
-      <c r="S21" s="47" t="s">
+      <c r="S21" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="T21" s="72" t="s">
+      <c r="T21" s="54" t="s">
         <v>266</v>
       </c>
-      <c r="U21" s="69" t="s">
+      <c r="U21" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="V21" s="67" t="s">
+      <c r="V21" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="W21" s="28" t="s">
+      <c r="W21" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="X21" s="39" t="s">
+      <c r="X21" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="Y21" s="39" t="s">
+      <c r="Y21" s="48" t="s">
         <v>732</v>
       </c>
-      <c r="Z21" s="39" t="s">
+      <c r="Z21" s="48" t="s">
         <v>733</v>
       </c>
-      <c r="AA21" s="39" t="s">
+      <c r="AA21" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="AB21" s="28" t="s">
+      <c r="AB21" s="46" t="s">
         <v>269</v>
       </c>
-      <c r="AC21" s="28" t="s">
+      <c r="AC21" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="AD21" s="28" t="s">
+      <c r="AD21" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="AE21" s="28" t="s">
+      <c r="AE21" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="AF21" s="28" t="s">
+      <c r="AF21" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="AG21" s="28" t="s">
+      <c r="AG21" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="AH21" s="39" t="s">
+      <c r="AH21" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="AI21" s="28" t="s">
+      <c r="AI21" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="AJ21" s="28" t="s">
+      <c r="AJ21" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="AK21" s="28" t="s">
+      <c r="AK21" s="46" t="s">
         <v>271</v>
       </c>
-      <c r="AL21" s="28" t="s">
+      <c r="AL21" s="46" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:38">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="73"/>
-      <c r="U22" s="70"/>
-      <c r="V22" s="68"/>
-      <c r="W22" s="28"/>
-      <c r="X22" s="66"/>
-      <c r="Y22" s="66"/>
-      <c r="Z22" s="66"/>
-      <c r="AA22" s="66"/>
-      <c r="AB22" s="28"/>
-      <c r="AC22" s="28"/>
-      <c r="AD22" s="28"/>
-      <c r="AE22" s="28"/>
-      <c r="AF22" s="28"/>
-      <c r="AG22" s="28"/>
-      <c r="AH22" s="39"/>
-      <c r="AI22" s="28"/>
-      <c r="AJ22" s="28"/>
-      <c r="AK22" s="28"/>
-      <c r="AL22" s="28"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="59"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="60"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="46"/>
+      <c r="AD22" s="46"/>
+      <c r="AE22" s="46"/>
+      <c r="AF22" s="46"/>
+      <c r="AG22" s="46"/>
+      <c r="AH22" s="48"/>
+      <c r="AI22" s="46"/>
+      <c r="AJ22" s="46"/>
+      <c r="AK22" s="46"/>
+      <c r="AL22" s="46"/>
     </row>
     <row r="23" spans="1:38">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="73"/>
-      <c r="U23" s="70"/>
-      <c r="V23" s="68"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="66"/>
-      <c r="Y23" s="66"/>
-      <c r="Z23" s="66"/>
-      <c r="AA23" s="66"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-      <c r="AG23" s="28"/>
-      <c r="AH23" s="39"/>
-      <c r="AI23" s="28"/>
-      <c r="AJ23" s="28"/>
-      <c r="AK23" s="28"/>
-      <c r="AL23" s="28"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="59"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="46"/>
+      <c r="AE23" s="46"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="46"/>
+      <c r="AH23" s="48"/>
+      <c r="AI23" s="46"/>
+      <c r="AJ23" s="46"/>
+      <c r="AK23" s="46"/>
+      <c r="AL23" s="46"/>
     </row>
     <row r="24" spans="1:38">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="73"/>
-      <c r="U24" s="70"/>
-      <c r="V24" s="68"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="66"/>
-      <c r="Y24" s="66"/>
-      <c r="Z24" s="66"/>
-      <c r="AA24" s="66"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
-      <c r="AG24" s="28"/>
-      <c r="AH24" s="39"/>
-      <c r="AI24" s="28"/>
-      <c r="AJ24" s="28"/>
-      <c r="AK24" s="28"/>
-      <c r="AL24" s="28"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="60"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
+      <c r="AD24" s="46"/>
+      <c r="AE24" s="46"/>
+      <c r="AF24" s="46"/>
+      <c r="AG24" s="46"/>
+      <c r="AH24" s="48"/>
+      <c r="AI24" s="46"/>
+      <c r="AJ24" s="46"/>
+      <c r="AK24" s="46"/>
+      <c r="AL24" s="46"/>
     </row>
     <row r="25" spans="1:38">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="70"/>
-      <c r="V25" s="68"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="66"/>
-      <c r="Y25" s="66"/>
-      <c r="Z25" s="66"/>
-      <c r="AA25" s="66"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="28"/>
-      <c r="AH25" s="39"/>
-      <c r="AI25" s="28"/>
-      <c r="AJ25" s="28"/>
-      <c r="AK25" s="28"/>
-      <c r="AL25" s="28"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="55"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46"/>
+      <c r="AD25" s="46"/>
+      <c r="AE25" s="46"/>
+      <c r="AF25" s="46"/>
+      <c r="AG25" s="46"/>
+      <c r="AH25" s="48"/>
+      <c r="AI25" s="46"/>
+      <c r="AJ25" s="46"/>
+      <c r="AK25" s="46"/>
+      <c r="AL25" s="46"/>
     </row>
     <row r="26" spans="1:38">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="73"/>
-      <c r="U26" s="70"/>
-      <c r="V26" s="68"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="66"/>
-      <c r="Y26" s="66"/>
-      <c r="Z26" s="66"/>
-      <c r="AA26" s="66"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="28"/>
-      <c r="AH26" s="39"/>
-      <c r="AI26" s="28"/>
-      <c r="AJ26" s="28"/>
-      <c r="AK26" s="28"/>
-      <c r="AL26" s="28"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="60"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="46"/>
+      <c r="AD26" s="46"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="46"/>
+      <c r="AH26" s="48"/>
+      <c r="AI26" s="46"/>
+      <c r="AJ26" s="46"/>
+      <c r="AK26" s="46"/>
+      <c r="AL26" s="46"/>
     </row>
     <row r="27" spans="1:38">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="73"/>
-      <c r="U27" s="70"/>
-      <c r="V27" s="68"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="66"/>
-      <c r="Y27" s="66"/>
-      <c r="Z27" s="66"/>
-      <c r="AA27" s="66"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="28"/>
-      <c r="AD27" s="28"/>
-      <c r="AE27" s="28"/>
-      <c r="AF27" s="28"/>
-      <c r="AG27" s="28"/>
-      <c r="AH27" s="39"/>
-      <c r="AI27" s="28"/>
-      <c r="AJ27" s="28"/>
-      <c r="AK27" s="28"/>
-      <c r="AL27" s="28"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="57"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="60"/>
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="46"/>
+      <c r="AD27" s="46"/>
+      <c r="AE27" s="46"/>
+      <c r="AF27" s="46"/>
+      <c r="AG27" s="46"/>
+      <c r="AH27" s="48"/>
+      <c r="AI27" s="46"/>
+      <c r="AJ27" s="46"/>
+      <c r="AK27" s="46"/>
+      <c r="AL27" s="46"/>
     </row>
     <row r="28" spans="1:38">
       <c r="R28" s="4"/>
-      <c r="U28" s="70"/>
+      <c r="U28" s="59"/>
       <c r="V28" s="1"/>
       <c r="X28" s="4"/>
       <c r="Y28" s="1"/>
@@ -10149,7 +10149,7 @@
       <c r="AI28" s="1"/>
     </row>
     <row r="29" spans="1:38" ht="90">
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="46" t="s">
         <v>233</v>
       </c>
       <c r="F29" s="22" t="s">
@@ -10159,7 +10159,7 @@
       <c r="T29" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="U29" s="70"/>
+      <c r="U29" s="59"/>
       <c r="V29" s="1"/>
       <c r="X29" s="4"/>
       <c r="Y29" s="1"/>
@@ -10177,7 +10177,7 @@
       <c r="AI29" s="1"/>
     </row>
     <row r="30" spans="1:38">
-      <c r="D30" s="28"/>
+      <c r="D30" s="46"/>
       <c r="R30" s="4"/>
       <c r="V30" s="1"/>
       <c r="X30" s="4"/>
@@ -10188,7 +10188,7 @@
       <c r="AI30" s="1"/>
     </row>
     <row r="31" spans="1:38" ht="11.25" customHeight="1">
-      <c r="D31" s="28"/>
+      <c r="D31" s="46"/>
       <c r="R31" s="4"/>
       <c r="T31" s="27" t="s">
         <v>267</v>
@@ -10198,7 +10198,7 @@
       <c r="Y31" s="1"/>
       <c r="AB31" s="4"/>
       <c r="AD31" s="2"/>
-      <c r="AF31" s="50" t="s">
+      <c r="AF31" s="31" t="s">
         <v>736</v>
       </c>
       <c r="AG31" s="11" t="s">
@@ -10207,7 +10207,7 @@
       <c r="AI31" s="1"/>
     </row>
     <row r="32" spans="1:38">
-      <c r="D32" s="28"/>
+      <c r="D32" s="46"/>
       <c r="R32" s="4"/>
       <c r="T32" s="27"/>
       <c r="V32" s="1"/>
@@ -10215,14 +10215,14 @@
       <c r="Y32" s="1"/>
       <c r="AB32" s="4"/>
       <c r="AD32" s="2"/>
-      <c r="AF32" s="50"/>
+      <c r="AF32" s="31"/>
       <c r="AG32" s="11" t="s">
         <v>277</v>
       </c>
       <c r="AI32" s="1"/>
     </row>
     <row r="33" spans="4:35">
-      <c r="D33" s="28"/>
+      <c r="D33" s="46"/>
       <c r="R33" s="4"/>
       <c r="T33" s="27"/>
       <c r="V33" s="1"/>
@@ -10230,14 +10230,14 @@
       <c r="Y33" s="1"/>
       <c r="AB33" s="4"/>
       <c r="AD33" s="2"/>
-      <c r="AF33" s="50"/>
+      <c r="AF33" s="31"/>
       <c r="AG33" s="11" t="s">
         <v>278</v>
       </c>
       <c r="AI33" s="1"/>
     </row>
     <row r="34" spans="4:35">
-      <c r="D34" s="28"/>
+      <c r="D34" s="46"/>
       <c r="N34" s="1"/>
       <c r="P34" s="4"/>
       <c r="T34" s="27"/>
@@ -10248,7 +10248,7 @@
       <c r="Y34" s="1"/>
       <c r="AB34" s="4"/>
       <c r="AC34" s="2"/>
-      <c r="AF34" s="50"/>
+      <c r="AF34" s="31"/>
       <c r="AG34" s="11" t="s">
         <v>279</v>
       </c>
@@ -10256,7 +10256,7 @@
       <c r="AI34" s="1"/>
     </row>
     <row r="35" spans="4:35">
-      <c r="D35" s="28"/>
+      <c r="D35" s="46"/>
       <c r="N35" s="1"/>
       <c r="P35" s="4"/>
       <c r="T35" s="27"/>
@@ -10267,7 +10267,7 @@
       <c r="Y35" s="1"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="2"/>
-      <c r="AF35" s="50"/>
+      <c r="AF35" s="31"/>
       <c r="AG35" s="11" t="s">
         <v>280</v>
       </c>
@@ -10285,7 +10285,7 @@
       <c r="Y36" s="1"/>
       <c r="AB36" s="4"/>
       <c r="AC36" s="2"/>
-      <c r="AF36" s="50"/>
+      <c r="AF36" s="31"/>
       <c r="AG36" s="11" t="s">
         <v>281</v>
       </c>
@@ -10304,7 +10304,7 @@
       <c r="Z37" s="4"/>
       <c r="AB37" s="4"/>
       <c r="AC37" s="2"/>
-      <c r="AF37" s="50"/>
+      <c r="AF37" s="31"/>
       <c r="AG37" s="11" t="s">
         <v>282</v>
       </c>
@@ -10323,7 +10323,7 @@
       <c r="Z38" s="4"/>
       <c r="AB38" s="4"/>
       <c r="AC38" s="2"/>
-      <c r="AF38" s="50"/>
+      <c r="AF38" s="31"/>
       <c r="AG38" s="11" t="s">
         <v>283</v>
       </c>
@@ -10342,7 +10342,7 @@
       <c r="Z39" s="4"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="2"/>
-      <c r="AF39" s="50"/>
+      <c r="AF39" s="31"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
     </row>
@@ -10358,7 +10358,7 @@
       <c r="Z40" s="4"/>
       <c r="AB40" s="4"/>
       <c r="AC40" s="2"/>
-      <c r="AF40" s="50"/>
+      <c r="AF40" s="31"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
     </row>
@@ -10374,7 +10374,7 @@
       <c r="Z41" s="4"/>
       <c r="AB41" s="4"/>
       <c r="AC41" s="2"/>
-      <c r="AF41" s="50"/>
+      <c r="AF41" s="31"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
     </row>
@@ -10383,39 +10383,39 @@
     </row>
     <row r="43" spans="4:35">
       <c r="Z43" s="4"/>
-      <c r="AF43" s="55" t="s">
+      <c r="AF43" s="63" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="44" spans="4:35">
       <c r="Z44" s="4"/>
-      <c r="AF44" s="55"/>
+      <c r="AF44" s="63"/>
     </row>
     <row r="45" spans="4:35">
       <c r="Z45" s="4"/>
-      <c r="AF45" s="55"/>
+      <c r="AF45" s="63"/>
     </row>
     <row r="46" spans="4:35">
       <c r="Z46" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="D29:D35"/>
-    <mergeCell ref="T21:T27"/>
-    <mergeCell ref="T31:T36"/>
-    <mergeCell ref="N21:N27"/>
-    <mergeCell ref="P21:P27"/>
-    <mergeCell ref="Q21:Q27"/>
-    <mergeCell ref="I21:I27"/>
-    <mergeCell ref="H21:H27"/>
-    <mergeCell ref="J21:J27"/>
-    <mergeCell ref="K21:K27"/>
-    <mergeCell ref="L21:L27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="S21:S27"/>
-    <mergeCell ref="E21:E27"/>
-    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="AH18:AH20"/>
+    <mergeCell ref="AF31:AF41"/>
+    <mergeCell ref="AF43:AF45"/>
+    <mergeCell ref="AG21:AG27"/>
+    <mergeCell ref="O21:O27"/>
+    <mergeCell ref="X18:AG20"/>
+    <mergeCell ref="W21:W27"/>
+    <mergeCell ref="G18:W20"/>
+    <mergeCell ref="AJ21:AJ27"/>
+    <mergeCell ref="AK21:AK27"/>
+    <mergeCell ref="AL21:AL27"/>
+    <mergeCell ref="X21:X27"/>
+    <mergeCell ref="AB21:AB27"/>
+    <mergeCell ref="Y21:Y27"/>
+    <mergeCell ref="AI21:AI27"/>
+    <mergeCell ref="AH21:AH27"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="V21:V27"/>
@@ -10432,22 +10432,22 @@
     <mergeCell ref="D21:D27"/>
     <mergeCell ref="F21:F27"/>
     <mergeCell ref="A18:F20"/>
-    <mergeCell ref="AJ21:AJ27"/>
-    <mergeCell ref="AK21:AK27"/>
-    <mergeCell ref="AL21:AL27"/>
-    <mergeCell ref="X21:X27"/>
-    <mergeCell ref="AB21:AB27"/>
-    <mergeCell ref="Y21:Y27"/>
-    <mergeCell ref="AI21:AI27"/>
-    <mergeCell ref="AH21:AH27"/>
-    <mergeCell ref="AH18:AH20"/>
-    <mergeCell ref="AF31:AF41"/>
-    <mergeCell ref="AF43:AF45"/>
-    <mergeCell ref="AG21:AG27"/>
-    <mergeCell ref="O21:O27"/>
-    <mergeCell ref="X18:AG20"/>
-    <mergeCell ref="W21:W27"/>
-    <mergeCell ref="G18:W20"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="S21:S27"/>
+    <mergeCell ref="E21:E27"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="D29:D35"/>
+    <mergeCell ref="T21:T27"/>
+    <mergeCell ref="T31:T36"/>
+    <mergeCell ref="N21:N27"/>
+    <mergeCell ref="P21:P27"/>
+    <mergeCell ref="Q21:Q27"/>
+    <mergeCell ref="I21:I27"/>
+    <mergeCell ref="H21:H27"/>
+    <mergeCell ref="J21:J27"/>
+    <mergeCell ref="K21:K27"/>
+    <mergeCell ref="L21:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10528,10 +10528,10 @@
       <c r="AY1" s="1"/>
     </row>
     <row r="2" spans="1:54" ht="21">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="5" t="s">
         <v>286</v>
       </c>
@@ -10560,10 +10560,10 @@
       <c r="BB2" s="3"/>
     </row>
     <row r="3" spans="1:54" ht="21">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="5" t="s">
         <v>360</v>
       </c>
@@ -12015,324 +12015,324 @@
       <c r="AG21" s="79"/>
     </row>
     <row r="22" spans="1:52" ht="11.25" customHeight="1">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="46" t="s">
         <v>336</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="46" t="s">
         <v>318</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="46" t="s">
         <v>319</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="46" t="s">
         <v>333</v>
       </c>
-      <c r="J22" s="28" t="s">
+      <c r="J22" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="K22" s="28" t="s">
+      <c r="K22" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="L22" s="28" t="s">
+      <c r="L22" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="M22" s="28" t="s">
+      <c r="M22" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="N22" s="28" t="s">
+      <c r="N22" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="O22" s="28" t="s">
+      <c r="O22" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="P22" s="28" t="s">
+      <c r="P22" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="Q22" s="28" t="s">
+      <c r="Q22" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="R22" s="28" t="s">
+      <c r="R22" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="S22" s="28" t="s">
+      <c r="S22" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="T22" s="28" t="s">
+      <c r="T22" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="U22" s="28" t="s">
+      <c r="U22" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="V22" s="28" t="s">
+      <c r="V22" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="W22" s="28" t="s">
+      <c r="W22" s="46" t="s">
         <v>325</v>
       </c>
-      <c r="X22" s="28" t="s">
+      <c r="X22" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="Y22" s="28" t="s">
+      <c r="Y22" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="Z22" s="28" t="s">
+      <c r="Z22" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="AA22" s="28" t="s">
+      <c r="AA22" s="46" t="s">
         <v>352</v>
       </c>
-      <c r="AB22" s="28" t="s">
+      <c r="AB22" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="AC22" s="28" t="s">
+      <c r="AC22" s="46" t="s">
         <v>337</v>
       </c>
-      <c r="AD22" s="28" t="s">
+      <c r="AD22" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="AE22" s="28" t="s">
+      <c r="AE22" s="46" t="s">
         <v>332</v>
       </c>
-      <c r="AF22" s="28" t="s">
+      <c r="AF22" s="46" t="s">
         <v>358</v>
       </c>
-      <c r="AG22" s="45" t="s">
+      <c r="AG22" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="AH22" s="28" t="s">
+      <c r="AH22" s="46" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:52">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="28"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="28"/>
-      <c r="Z23" s="28"/>
-      <c r="AA23" s="28"/>
-      <c r="AB23" s="28"/>
-      <c r="AC23" s="28"/>
-      <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
-      <c r="AF23" s="28"/>
-      <c r="AG23" s="43"/>
-      <c r="AH23" s="28"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="46"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="46"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="46"/>
+      <c r="AE23" s="46"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="29"/>
+      <c r="AH23" s="46"/>
     </row>
     <row r="24" spans="1:52">
-      <c r="A24" s="46"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="28"/>
-      <c r="AA24" s="28"/>
-      <c r="AB24" s="28"/>
-      <c r="AC24" s="28"/>
-      <c r="AD24" s="28"/>
-      <c r="AE24" s="28"/>
-      <c r="AF24" s="28"/>
-      <c r="AG24" s="43"/>
-      <c r="AH24" s="28"/>
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="46"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="46"/>
+      <c r="V24" s="46"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="46"/>
+      <c r="Y24" s="46"/>
+      <c r="Z24" s="46"/>
+      <c r="AA24" s="46"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
+      <c r="AD24" s="46"/>
+      <c r="AE24" s="46"/>
+      <c r="AF24" s="46"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="46"/>
     </row>
     <row r="25" spans="1:52">
-      <c r="A25" s="46"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
-      <c r="Z25" s="28"/>
-      <c r="AA25" s="28"/>
-      <c r="AB25" s="28"/>
-      <c r="AC25" s="28"/>
-      <c r="AD25" s="28"/>
-      <c r="AE25" s="28"/>
-      <c r="AF25" s="28"/>
-      <c r="AG25" s="43"/>
-      <c r="AH25" s="28"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="46"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="46"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="46"/>
+      <c r="U25" s="46"/>
+      <c r="V25" s="46"/>
+      <c r="W25" s="46"/>
+      <c r="X25" s="46"/>
+      <c r="Y25" s="46"/>
+      <c r="Z25" s="46"/>
+      <c r="AA25" s="46"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46"/>
+      <c r="AD25" s="46"/>
+      <c r="AE25" s="46"/>
+      <c r="AF25" s="46"/>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="46"/>
     </row>
     <row r="26" spans="1:52">
-      <c r="A26" s="46"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="28"/>
-      <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="Y26" s="28"/>
-      <c r="Z26" s="28"/>
-      <c r="AA26" s="28"/>
-      <c r="AB26" s="28"/>
-      <c r="AC26" s="28"/>
-      <c r="AD26" s="28"/>
-      <c r="AE26" s="28"/>
-      <c r="AF26" s="28"/>
-      <c r="AG26" s="43"/>
-      <c r="AH26" s="28"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="46"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="46"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="46"/>
+      <c r="U26" s="46"/>
+      <c r="V26" s="46"/>
+      <c r="W26" s="46"/>
+      <c r="X26" s="46"/>
+      <c r="Y26" s="46"/>
+      <c r="Z26" s="46"/>
+      <c r="AA26" s="46"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="46"/>
+      <c r="AD26" s="46"/>
+      <c r="AE26" s="46"/>
+      <c r="AF26" s="46"/>
+      <c r="AG26" s="29"/>
+      <c r="AH26" s="46"/>
     </row>
     <row r="27" spans="1:52">
-      <c r="A27" s="46"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
-      <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="Y27" s="28"/>
-      <c r="Z27" s="28"/>
-      <c r="AA27" s="28"/>
-      <c r="AB27" s="28"/>
-      <c r="AC27" s="28"/>
-      <c r="AD27" s="28"/>
-      <c r="AE27" s="28"/>
-      <c r="AF27" s="28"/>
-      <c r="AG27" s="43"/>
-      <c r="AH27" s="28"/>
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+      <c r="U27" s="46"/>
+      <c r="V27" s="46"/>
+      <c r="W27" s="46"/>
+      <c r="X27" s="46"/>
+      <c r="Y27" s="46"/>
+      <c r="Z27" s="46"/>
+      <c r="AA27" s="46"/>
+      <c r="AB27" s="46"/>
+      <c r="AC27" s="46"/>
+      <c r="AD27" s="46"/>
+      <c r="AE27" s="46"/>
+      <c r="AF27" s="46"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="46"/>
     </row>
     <row r="28" spans="1:52">
-      <c r="A28" s="47"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="28"/>
-      <c r="V28" s="28"/>
-      <c r="W28" s="28"/>
-      <c r="X28" s="28"/>
-      <c r="Y28" s="28"/>
-      <c r="Z28" s="28"/>
-      <c r="AA28" s="28"/>
-      <c r="AB28" s="28"/>
-      <c r="AC28" s="28"/>
-      <c r="AD28" s="28"/>
-      <c r="AE28" s="28"/>
-      <c r="AF28" s="28"/>
-      <c r="AG28" s="44"/>
-      <c r="AH28" s="28"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+      <c r="U28" s="46"/>
+      <c r="V28" s="46"/>
+      <c r="W28" s="46"/>
+      <c r="X28" s="46"/>
+      <c r="Y28" s="46"/>
+      <c r="Z28" s="46"/>
+      <c r="AA28" s="46"/>
+      <c r="AB28" s="46"/>
+      <c r="AC28" s="46"/>
+      <c r="AD28" s="46"/>
+      <c r="AE28" s="46"/>
+      <c r="AF28" s="46"/>
+      <c r="AG28" s="30"/>
+      <c r="AH28" s="46"/>
     </row>
     <row r="29" spans="1:52">
       <c r="D29" s="4"/>
@@ -12341,16 +12341,16 @@
     </row>
     <row r="30" spans="1:52" ht="11.25" customHeight="1">
       <c r="D30" s="4"/>
-      <c r="I30" s="42" t="s">
+      <c r="I30" s="28" t="s">
         <v>335</v>
       </c>
-      <c r="W30" s="28" t="s">
+      <c r="W30" s="46" t="s">
         <v>326</v>
       </c>
-      <c r="Y30" s="39" t="s">
+      <c r="Y30" s="48" t="s">
         <v>326</v>
       </c>
-      <c r="Z30" s="39" t="s">
+      <c r="Z30" s="48" t="s">
         <v>326</v>
       </c>
       <c r="AE30" s="18" t="s">
@@ -12359,50 +12359,50 @@
     </row>
     <row r="31" spans="1:52">
       <c r="D31" s="4"/>
-      <c r="I31" s="46"/>
-      <c r="W31" s="28"/>
-      <c r="Y31" s="39"/>
-      <c r="Z31" s="39"/>
+      <c r="I31" s="44"/>
+      <c r="W31" s="46"/>
+      <c r="Y31" s="48"/>
+      <c r="Z31" s="48"/>
       <c r="AE31" s="19" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:52" ht="11.25" customHeight="1">
       <c r="D32" s="4"/>
-      <c r="I32" s="46"/>
-      <c r="W32" s="28"/>
-      <c r="Y32" s="39"/>
-      <c r="Z32" s="39"/>
+      <c r="I32" s="44"/>
+      <c r="W32" s="46"/>
+      <c r="Y32" s="48"/>
+      <c r="Z32" s="48"/>
       <c r="AE32" s="19" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="33" spans="4:31">
       <c r="D33" s="4"/>
-      <c r="I33" s="46"/>
-      <c r="W33" s="28"/>
-      <c r="Y33" s="39"/>
-      <c r="Z33" s="39"/>
+      <c r="I33" s="44"/>
+      <c r="W33" s="46"/>
+      <c r="Y33" s="48"/>
+      <c r="Z33" s="48"/>
       <c r="AE33" s="19" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="34" spans="4:31">
       <c r="D34" s="4"/>
-      <c r="I34" s="46"/>
-      <c r="W34" s="28"/>
-      <c r="Y34" s="39"/>
-      <c r="Z34" s="39"/>
+      <c r="I34" s="44"/>
+      <c r="W34" s="46"/>
+      <c r="Y34" s="48"/>
+      <c r="Z34" s="48"/>
       <c r="AE34" s="19" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="35" spans="4:31">
       <c r="D35" s="4"/>
-      <c r="I35" s="47"/>
-      <c r="W35" s="28"/>
-      <c r="Y35" s="39"/>
-      <c r="Z35" s="39"/>
+      <c r="I35" s="45"/>
+      <c r="W35" s="46"/>
+      <c r="Y35" s="48"/>
+      <c r="Z35" s="48"/>
       <c r="AE35" s="20" t="s">
         <v>331</v>
       </c>
@@ -12415,68 +12415,97 @@
     </row>
     <row r="37" spans="4:31" ht="11.25" customHeight="1">
       <c r="D37" s="4"/>
-      <c r="W37" s="42" t="s">
+      <c r="W37" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="Y37" s="45" t="s">
+      <c r="Y37" s="43" t="s">
         <v>342</v>
       </c>
-      <c r="Z37" s="45" t="s">
+      <c r="Z37" s="43" t="s">
         <v>343</v>
       </c>
       <c r="AE37" s="1"/>
     </row>
     <row r="38" spans="4:31">
       <c r="D38" s="4"/>
-      <c r="W38" s="46"/>
+      <c r="W38" s="44"/>
       <c r="Y38" s="89"/>
       <c r="Z38" s="89"/>
       <c r="AE38" s="1"/>
     </row>
     <row r="39" spans="4:31">
       <c r="D39" s="4"/>
-      <c r="W39" s="46"/>
+      <c r="W39" s="44"/>
       <c r="Y39" s="89"/>
       <c r="Z39" s="89"/>
       <c r="AE39" s="1"/>
     </row>
     <row r="40" spans="4:31">
       <c r="D40" s="4"/>
-      <c r="W40" s="46"/>
+      <c r="W40" s="44"/>
       <c r="Y40" s="89"/>
       <c r="Z40" s="89"/>
       <c r="AE40" s="1"/>
     </row>
     <row r="41" spans="4:31">
       <c r="D41" s="4"/>
-      <c r="W41" s="46"/>
+      <c r="W41" s="44"/>
       <c r="Y41" s="89"/>
       <c r="Z41" s="89"/>
       <c r="AE41" s="1"/>
     </row>
     <row r="42" spans="4:31">
       <c r="D42" s="4"/>
-      <c r="W42" s="46"/>
+      <c r="W42" s="44"/>
       <c r="Y42" s="89"/>
       <c r="Z42" s="89"/>
       <c r="AE42" s="1"/>
     </row>
     <row r="43" spans="4:31">
       <c r="D43" s="4"/>
-      <c r="W43" s="46"/>
+      <c r="W43" s="44"/>
       <c r="Y43" s="89"/>
       <c r="Z43" s="89"/>
       <c r="AE43" s="1"/>
     </row>
     <row r="44" spans="4:31">
       <c r="D44" s="4"/>
-      <c r="W44" s="47"/>
+      <c r="W44" s="45"/>
       <c r="Y44" s="90"/>
       <c r="Z44" s="90"/>
       <c r="AE44" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="AF19:AG21"/>
+    <mergeCell ref="A19:AE21"/>
+    <mergeCell ref="W37:W44"/>
+    <mergeCell ref="Y37:Y44"/>
+    <mergeCell ref="X22:X28"/>
+    <mergeCell ref="Z22:Z28"/>
+    <mergeCell ref="Z30:Z35"/>
+    <mergeCell ref="Z37:Z44"/>
+    <mergeCell ref="AE22:AE28"/>
+    <mergeCell ref="I22:I28"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="I30:I35"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="Y22:Y28"/>
+    <mergeCell ref="Y30:Y35"/>
+    <mergeCell ref="C22:C28"/>
+    <mergeCell ref="G22:G28"/>
+    <mergeCell ref="H22:H28"/>
+    <mergeCell ref="M22:M28"/>
+    <mergeCell ref="J22:J28"/>
+    <mergeCell ref="K22:K28"/>
+    <mergeCell ref="L22:L28"/>
+    <mergeCell ref="AF22:AF28"/>
+    <mergeCell ref="AG22:AG28"/>
+    <mergeCell ref="AH22:AH28"/>
+    <mergeCell ref="AB22:AB28"/>
+    <mergeCell ref="AA22:AA28"/>
+    <mergeCell ref="AC22:AC28"/>
+    <mergeCell ref="AD22:AD28"/>
     <mergeCell ref="N22:N28"/>
     <mergeCell ref="A22:A28"/>
     <mergeCell ref="A2:B2"/>
@@ -12493,35 +12522,6 @@
     <mergeCell ref="T22:T28"/>
     <mergeCell ref="E22:E28"/>
     <mergeCell ref="F22:F28"/>
-    <mergeCell ref="AF22:AF28"/>
-    <mergeCell ref="AG22:AG28"/>
-    <mergeCell ref="AH22:AH28"/>
-    <mergeCell ref="AB22:AB28"/>
-    <mergeCell ref="AA22:AA28"/>
-    <mergeCell ref="AC22:AC28"/>
-    <mergeCell ref="AD22:AD28"/>
-    <mergeCell ref="G22:G28"/>
-    <mergeCell ref="H22:H28"/>
-    <mergeCell ref="M22:M28"/>
-    <mergeCell ref="J22:J28"/>
-    <mergeCell ref="K22:K28"/>
-    <mergeCell ref="L22:L28"/>
-    <mergeCell ref="AF19:AG21"/>
-    <mergeCell ref="A19:AE21"/>
-    <mergeCell ref="W37:W44"/>
-    <mergeCell ref="Y37:Y44"/>
-    <mergeCell ref="X22:X28"/>
-    <mergeCell ref="Z22:Z28"/>
-    <mergeCell ref="Z30:Z35"/>
-    <mergeCell ref="Z37:Z44"/>
-    <mergeCell ref="AE22:AE28"/>
-    <mergeCell ref="I22:I28"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="I30:I35"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="Y22:Y28"/>
-    <mergeCell ref="Y30:Y35"/>
-    <mergeCell ref="C22:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>